<commit_message>
working on spinner progress bar
</commit_message>
<xml_diff>
--- a/TaskSummary.xlsx
+++ b/TaskSummary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammad.umerkhan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\AndroidStudioProjects\UploadFilesWithRetrofit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
   <si>
     <t>E-Commerce</t>
   </si>
@@ -290,6 +290,15 @@
       <t xml:space="preserve">
  </t>
     </r>
+  </si>
+  <si>
+    <t>16 April, 209</t>
+  </si>
+  <si>
+    <t>Working on Spinner Progress Bar</t>
+  </si>
+  <si>
+    <t>16 April, 2019</t>
   </si>
 </sst>
 </file>
@@ -945,7 +954,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1000,6 +1009,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="0" xfId="44" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="30" borderId="0" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1009,13 +1027,7 @@
     <xf numFmtId="0" fontId="25" fillId="31" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="0" xfId="44" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1737,10 +1749,10 @@
       <c r="AG4" s="9"/>
     </row>
     <row r="5" spans="1:33">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="22"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -3141,10 +3153,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3156,30 +3168,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="13" t="s">
@@ -3307,7 +3319,7 @@
       <c r="A16" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="23" t="s">
         <v>79</v>
       </c>
       <c r="C16" s="20" t="s">
@@ -3318,11 +3330,22 @@
       <c r="A17" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="24" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3601,20 +3624,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Process_x0020_Area xmlns="0e054974-4a2e-4650-8bee-77d4a4f03c7d">Process and Product Quality Assurance</Process_x0020_Area>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Process_x0020_Area xmlns="0e054974-4a2e-4650-8bee-77d4a4f03c7d">Process and Product Quality Assurance</Process_x0020_Area>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3761,14 +3784,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67584ED9-A85A-42A0-8E69-9AEEF31F9126}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A182D93-DA67-4246-9C70-86C0D94565C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3780,6 +3795,14 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67584ED9-A85A-42A0-8E69-9AEEF31F9126}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>